<commit_message>
Update HealthProfessional mapping regarding the role
</commit_message>
<xml_diff>
--- a/maps/HealthProfessional.xlsx
+++ b/maps/HealthProfessional.xlsx
@@ -61,22 +61,22 @@
     <t xml:space="preserve">EHDSHealthProfessional.role</t>
   </si>
   <si>
+    <t xml:space="preserve">EHDSHealthProfessional.organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthProfessional.HealthcareProvider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EHDSHealthProfessional.specialty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthProfessional.Specialty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthProfessional.Gender</t>
+  </si>
+  <si>
     <t xml:space="preserve">HealthProfessional.HealthProfessionalRole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EHDSHealthProfessional.organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HealthProfessional.HealthcareProvider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EHDSHealthProfessional.specialty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HealthProfessional.Specialty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HealthProfessional.Gender</t>
   </si>
 </sst>
 </file>
@@ -365,7 +365,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -425,28 +425,30 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>